<commit_message>
ultimos cambios y q Dios nos agarre confesados
</commit_message>
<xml_diff>
--- a/Back-End/estudiantes_seccion_1.xlsx
+++ b/Back-End/estudiantes_seccion_1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Primer Nombre</t>
   </si>
@@ -32,27 +32,6 @@
   </si>
   <si>
     <t>Hora</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>20181002386</t>
-  </si>
-  <si>
-    <t>Bases</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>20201001234</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>20181002200</t>
   </si>
 </sst>
 </file>
@@ -429,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="8" width="15" customWidth="1"/>
@@ -461,84 +440,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>1000</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>